<commit_message>
Correction des choix de promo dans l'onglet Groupes des database file
</commit_message>
<xml_diff>
--- a/FlOpEDT/misc/deploy_database/database_file.xlsx
+++ b/FlOpEDT/misc/deploy_database/database_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Intervenants" sheetId="1" state="visible" r:id="rId2"/>
@@ -305,7 +305,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -369,12 +369,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -507,7 +501,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -592,10 +586,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -612,7 +602,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -628,23 +618,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -731,21 +721,18 @@
   </sheetPr>
   <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="8.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.22"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,7 +2025,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2053,18 +2040,18 @@
   </sheetPr>
   <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2735,7 +2722,7 @@
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13"/>
       <c r="B32" s="14"/>
-      <c r="E32" s="21"/>
+      <c r="E32" s="20"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
@@ -2959,7 +2946,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -2974,209 +2961,209 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="27.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="M1" s="22" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="M1" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="22"/>
+      <c r="N1" s="21"/>
     </row>
     <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="M2" s="23" t="s">
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="M2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="O2" s="25" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13"/>
       <c r="B3" s="7"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
-      <c r="O3" s="28" t="s">
+      <c r="O3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="P3" s="27" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13"/>
       <c r="B4" s="7"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
       <c r="M4" s="13"/>
       <c r="N4" s="13"/>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="P4" s="28" t="s">
+      <c r="P4" s="27" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="25" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13"/>
       <c r="B7" s="7"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13"/>
       <c r="B8" s="7"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13"/>
       <c r="B9" s="7"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13"/>
       <c r="B10" s="7"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="G10" s="22" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="G10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="21"/>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="G11" s="23" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="G11" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="25" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="27" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13"/>
       <c r="B13" s="7"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
@@ -3184,9 +3171,9 @@
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -3194,71 +3181,71 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
-      <c r="M15" s="22" t="s">
+      <c r="M15" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13"/>
       <c r="B16" s="7"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
-      <c r="M16" s="23" t="s">
+      <c r="M16" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="N16" s="26" t="s">
+      <c r="N16" s="25" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13"/>
       <c r="B17" s="7"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="M17" s="13"/>
-      <c r="N17" s="28" t="s">
+      <c r="N17" s="27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
       <c r="M18" s="13"/>
-      <c r="N18" s="28" t="s">
+      <c r="N18" s="27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="28" t="s">
+      <c r="N19" s="27" t="s">
         <v>47</v>
       </c>
       <c r="O19" s="0" t="s">
@@ -3268,11 +3255,11 @@
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13"/>
       <c r="B20" s="7"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
       <c r="M20" s="13"/>
-      <c r="N20" s="28" t="s">
+      <c r="N20" s="27" t="s">
         <v>49</v>
       </c>
       <c r="O20" s="0" t="s">
@@ -3282,11 +3269,11 @@
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13"/>
       <c r="B21" s="7"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
       <c r="M21" s="13"/>
-      <c r="N21" s="28" t="s">
+      <c r="N21" s="27" t="s">
         <v>51</v>
       </c>
       <c r="O21" s="0" t="s">
@@ -3296,78 +3283,74 @@
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13"/>
       <c r="B22" s="7"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
       <c r="M22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13"/>
       <c r="B23" s="7"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
       <c r="M23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
       <c r="M24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13"/>
       <c r="B25" s="7"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
       <c r="M25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13"/>
       <c r="B26" s="7"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
       <c r="M26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13"/>
       <c r="B27" s="7"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
       <c r="M27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13"/>
       <c r="B28" s="7"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13"/>
       <c r="B29" s="7"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B30" type="list">
-      <formula1>Modules!$M$3:$M$20</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C3:D30" type="list">
       <formula1>Groupes!$A$3:$A$30</formula1>
       <formula2>0</formula2>
@@ -3376,10 +3359,14 @@
       <formula1>Groupes!$M$17:$M$27</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:B30" type="list">
+      <formula1>Groupes!$M$3:$M$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -3394,20 +3381,20 @@
   </sheetPr>
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="61.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3435,7 +3422,7 @@
       <c r="E2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="23" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3443,9 +3430,9 @@
       <c r="A3" s="13"/>
       <c r="B3" s="7"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
       <c r="H3" s="1" t="s">
         <v>59</v>
       </c>
@@ -3456,9 +3443,9 @@
       <c r="A4" s="13"/>
       <c r="B4" s="6"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
       <c r="H4" s="1" t="s">
         <v>60</v>
       </c>
@@ -3469,481 +3456,481 @@
       <c r="A5" s="13"/>
       <c r="B5" s="6"/>
       <c r="C5" s="13"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13"/>
       <c r="B6" s="6"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13"/>
       <c r="B7" s="6"/>
       <c r="C7" s="13"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13"/>
       <c r="B8" s="6"/>
       <c r="C8" s="13"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13"/>
       <c r="B9" s="6"/>
       <c r="C9" s="13"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13"/>
       <c r="B10" s="6"/>
       <c r="C10" s="13"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13"/>
       <c r="B11" s="6"/>
       <c r="C11" s="13"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13"/>
       <c r="B12" s="6"/>
       <c r="C12" s="13"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13"/>
       <c r="B13" s="6"/>
       <c r="C13" s="13"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13"/>
       <c r="B14" s="6"/>
       <c r="C14" s="13"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13"/>
       <c r="B15" s="6"/>
       <c r="C15" s="13"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13"/>
       <c r="B16" s="6"/>
       <c r="C16" s="13"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13"/>
       <c r="B17" s="6"/>
       <c r="C17" s="13"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13"/>
       <c r="B18" s="6"/>
       <c r="C18" s="13"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13"/>
       <c r="B19" s="6"/>
       <c r="C19" s="13"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13"/>
       <c r="B20" s="6"/>
       <c r="C20" s="13"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13"/>
       <c r="B21" s="6"/>
       <c r="C21" s="13"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="13"/>
       <c r="B22" s="6"/>
       <c r="C22" s="13"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="13"/>
       <c r="B23" s="6"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13"/>
       <c r="B24" s="6"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13"/>
       <c r="B25" s="6"/>
       <c r="C25" s="13"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13"/>
       <c r="B26" s="6"/>
       <c r="C26" s="13"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="13"/>
       <c r="B27" s="6"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="13"/>
       <c r="B28" s="6"/>
       <c r="C28" s="13"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="13"/>
       <c r="B29" s="6"/>
       <c r="C29" s="13"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="13"/>
       <c r="B30" s="6"/>
       <c r="C30" s="13"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="13"/>
       <c r="B31" s="6"/>
       <c r="C31" s="13"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="13"/>
       <c r="B32" s="6"/>
       <c r="C32" s="13"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="13"/>
       <c r="B33" s="6"/>
       <c r="C33" s="13"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="13"/>
       <c r="B34" s="6"/>
       <c r="C34" s="13"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="13"/>
       <c r="B35" s="6"/>
       <c r="C35" s="13"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="13"/>
       <c r="B36" s="6"/>
       <c r="C36" s="13"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="13"/>
       <c r="B37" s="6"/>
       <c r="C37" s="13"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="13"/>
       <c r="B38" s="6"/>
       <c r="C38" s="13"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="13"/>
       <c r="B39" s="6"/>
       <c r="C39" s="13"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="13"/>
       <c r="B40" s="6"/>
       <c r="C40" s="13"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="13"/>
       <c r="B41" s="6"/>
       <c r="C41" s="13"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="13"/>
       <c r="B42" s="6"/>
       <c r="C42" s="13"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="13"/>
       <c r="B43" s="6"/>
       <c r="C43" s="13"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="13"/>
       <c r="B44" s="6"/>
       <c r="C44" s="13"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="13"/>
       <c r="B45" s="6"/>
       <c r="C45" s="13"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="13"/>
       <c r="B46" s="6"/>
       <c r="C46" s="13"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="13"/>
       <c r="B47" s="6"/>
       <c r="C47" s="13"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="13"/>
       <c r="B48" s="6"/>
       <c r="C48" s="13"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="13"/>
       <c r="B49" s="6"/>
       <c r="C49" s="13"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="13"/>
       <c r="B50" s="6"/>
       <c r="C50" s="13"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="13"/>
       <c r="B51" s="6"/>
       <c r="C51" s="13"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="13"/>
       <c r="B52" s="6"/>
       <c r="C52" s="13"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="13"/>
       <c r="B53" s="6"/>
       <c r="C53" s="13"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="13"/>
       <c r="B54" s="6"/>
       <c r="C54" s="13"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="26"/>
+      <c r="F54" s="26"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="13"/>
       <c r="B55" s="6"/>
       <c r="C55" s="13"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="13"/>
       <c r="B56" s="6"/>
       <c r="C56" s="13"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="13"/>
       <c r="B57" s="6"/>
       <c r="C57" s="13"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="13"/>
       <c r="B58" s="6"/>
       <c r="C58" s="13"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="27"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="13"/>
       <c r="B59" s="6"/>
       <c r="C59" s="13"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="13"/>
       <c r="B60" s="6"/>
       <c r="C60" s="13"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="13"/>
       <c r="B61" s="6"/>
       <c r="C61" s="13"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="27"/>
-      <c r="F61" s="27"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="13"/>
       <c r="B62" s="6"/>
       <c r="C62" s="13"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="13"/>
       <c r="B63" s="6"/>
       <c r="C63" s="13"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="13"/>
       <c r="B64" s="6"/>
       <c r="C64" s="13"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -3966,7 +3953,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -3981,26 +3968,26 @@
   </sheetPr>
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="24.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.23979591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4015,10 +4002,10 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="30"/>
+      <c r="M1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
@@ -4037,216 +4024,216 @@
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="M2" s="30"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="L3" s="32" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="L3" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="M3" s="32"/>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="L4" s="30" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="L4" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="M4" s="30"/>
+      <c r="M4" s="29"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="L5" s="30" t="s">
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="L5" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="M5" s="30"/>
+      <c r="M5" s="29"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="31"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="L7" s="33" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="L7" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="L8" s="22" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="L8" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="L9" s="22" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="L9" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="M9" s="22" t="s">
+      <c r="M9" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="L10" s="22" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="L10" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="M10" s="22" t="s">
+      <c r="M10" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="L11" s="22" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="L11" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="M11" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="L12" s="22" t="s">
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="L12" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="M12" s="22" t="s">
+      <c r="M12" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="31"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
       <c r="L13" s="4" t="s">
         <v>63</v>
       </c>
@@ -4262,242 +4249,242 @@
       <c r="R13" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="L14" s="34" t="n">
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="L14" s="33" t="n">
         <v>90</v>
       </c>
-      <c r="M14" s="34" t="s">
+      <c r="M14" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="N14" s="35" t="s">
+      <c r="N14" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="O14" s="35" t="s">
+      <c r="O14" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="L15" s="34" t="n">
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="L15" s="33" t="n">
         <v>60</v>
       </c>
-      <c r="M15" s="34" t="s">
+      <c r="M15" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="N15" s="35" t="s">
+      <c r="N15" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="L16" s="34" t="n">
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="L16" s="33" t="n">
         <v>30</v>
       </c>
-      <c r="M16" s="34" t="s">
+      <c r="M16" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="N16" s="35" t="s">
+      <c r="N16" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="O16" s="35" t="s">
+      <c r="O16" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="L17" s="34" t="n">
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="L17" s="33" t="n">
         <v>45</v>
       </c>
-      <c r="M17" s="34" t="s">
+      <c r="M17" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="N17" s="35" t="s">
+      <c r="N17" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="O17" s="35" t="s">
+      <c r="O17" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="31"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
+      <c r="A22" s="30"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
+      <c r="A24" s="30"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
+      <c r="A27" s="30"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4531,7 +4518,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -4546,291 +4533,291 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.52"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="13"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="13"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="13"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="13"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="13"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="13"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="13"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="13"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="13"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="13"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="25" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28" t="s">
+      <c r="A25" s="27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4843,7 +4830,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
deploy database scripts no-slot
</commit_message>
<xml_diff>
--- a/FlOpEDT/misc/deploy_database/database_file.xlsx
+++ b/FlOpEDT/misc/deploy_database/database_file.xlsx
@@ -5,15 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Intervenants" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Salles" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Groupes" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Modules" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Creneaux" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Cours" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Cours" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Creneaux" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
   <si>
     <t xml:space="preserve">Liste intervenants</t>
   </si>
@@ -210,60 +210,78 @@
     <t xml:space="preserve">être entre 0 et 53</t>
   </si>
   <si>
+    <t xml:space="preserve">Liste des types de cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Durée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liste des Types de Groupes concernés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP90</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liste Créneaux</t>
   </si>
   <si>
     <t xml:space="preserve">Est-ce que votre département possède</t>
   </si>
   <si>
+    <t xml:space="preserve">Types de Cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horaires auxquels ce type de créneau peut commencer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniquement des créneaux de 1h30 ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oui</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si votre réponse est «Oui », </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ne remplissez pas les tableaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">« Je veux que les créneaux possibles soient :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De 90 minutes :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A partir de 8h et de 9h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De 60 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">à 8h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De 30 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le lundi à 10h30 et 11h45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De 45 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le mercredi à 11h15 ou 11h</t>
+  </si>
+  <si>
     <t xml:space="preserve">Durée (en min)</t>
   </si>
   <si>
-    <t xml:space="preserve">Jours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horaires auxquels ce type de créneau peut commencer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Uniquement des créneaux de 1h30 ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oui</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si votre réponse est «Oui », </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ne remplissez pas les tableaux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">« Je veux que les créneaux possibles soient :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De 90 minutes :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A partir de 8h et de 9h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De 60 min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">à 8h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De 30 min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le lundi à 10h30 et 11h45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">De 45 min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">le mercredi à 11h15 ou 11h</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tous les jours</t>
   </si>
   <si>
@@ -289,12 +307,6 @@
   </si>
   <si>
     <t xml:space="preserve">11h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liste des types de cours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liste des Types de Groupes concernés</t>
   </si>
 </sst>
 </file>
@@ -721,18 +733,21 @@
   </sheetPr>
   <dimension ref="A1:P95"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2857142857143"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2025,7 +2040,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -2040,18 +2055,18 @@
   </sheetPr>
   <dimension ref="A1:T75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2946,7 +2961,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -2961,28 +2976,28 @@
   </sheetPr>
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="27.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3366,7 +3381,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -3381,20 +3396,20 @@
   </sheetPr>
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="60.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3953,7 +3968,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
@@ -3966,33 +3981,384 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.37"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="26"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="25"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="27" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="27" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="27" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="27"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C3:K21" type="list">
+      <formula1>Groupes!$M$17:$M$27</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.23979591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="24.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="20" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4003,19 +4369,19 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="L1" s="29" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="M1" s="29"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
@@ -4025,7 +4391,7 @@
       <c r="I2" s="16"/>
       <c r="J2" s="16"/>
       <c r="L2" s="29" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="M2" s="29"/>
     </row>
@@ -4041,7 +4407,7 @@
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
       <c r="L3" s="31" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="M3" s="31"/>
     </row>
@@ -4057,7 +4423,7 @@
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
       <c r="L4" s="29" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="M4" s="29"/>
     </row>
@@ -4073,7 +4439,7 @@
       <c r="I5" s="28"/>
       <c r="J5" s="28"/>
       <c r="L5" s="29" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="M5" s="29"/>
     </row>
@@ -4122,7 +4488,7 @@
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="L8" s="21" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
@@ -4143,10 +4509,10 @@
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
       <c r="L9" s="21" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="N9" s="21"/>
       <c r="O9" s="21"/>
@@ -4166,10 +4532,10 @@
       <c r="I10" s="28"/>
       <c r="J10" s="28"/>
       <c r="L10" s="21" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="N10" s="21"/>
       <c r="O10" s="21"/>
@@ -4189,10 +4555,10 @@
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
       <c r="L11" s="21" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="M11" s="21" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="N11" s="21"/>
       <c r="O11" s="21"/>
@@ -4212,10 +4578,10 @@
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
       <c r="L12" s="21" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="M12" s="21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="N12" s="21"/>
       <c r="O12" s="21"/>
@@ -4235,13 +4601,13 @@
       <c r="I13" s="28"/>
       <c r="J13" s="28"/>
       <c r="L13" s="4" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="N13" s="16" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="O13" s="16"/>
       <c r="P13" s="16"/>
@@ -4263,13 +4629,13 @@
         <v>90</v>
       </c>
       <c r="M14" s="33" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="N14" s="34" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="O14" s="34" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
@@ -4290,10 +4656,10 @@
         <v>60</v>
       </c>
       <c r="M15" s="33" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="O15" s="34"/>
       <c r="P15" s="34"/>
@@ -4315,13 +4681,13 @@
         <v>30</v>
       </c>
       <c r="M16" s="33" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="O16" s="34" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="P16" s="34"/>
       <c r="Q16" s="34"/>
@@ -4342,13 +4708,13 @@
         <v>45</v>
       </c>
       <c r="M17" s="33" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="N17" s="34" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="O17" s="34" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="P17" s="34"/>
       <c r="Q17" s="34"/>
@@ -4518,319 +4884,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J26"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B3:J21" type="list">
-      <formula1>Groupes!$M$17:$M$27</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
add TimeGeneralSettings to import process
</commit_message>
<xml_diff>
--- a/FlOpEDT/misc/deploy_database/database_file.xlsx
+++ b/FlOpEDT/misc/deploy_database/database_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Intervenants" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Modules" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Groupes" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Cours" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Paramètres" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="92">
   <si>
     <t xml:space="preserve">Liste intervenants</t>
   </si>
@@ -255,15 +256,61 @@
   </si>
   <si>
     <t xml:space="preserve">TP240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horaires de fonctionnement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jours ouvrables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Début des cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lundi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mardi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercredi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeudi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendredi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samedi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimanche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fin des cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Début de la pause déjeuner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fin de la pause déjeuner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="HH:MM"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -498,7 +545,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -650,6 +697,26 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3468,7 +3535,7 @@
   </sheetPr>
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4079,4 +4146,129 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="38" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="42" t="n">
+        <v>0.333333333333333</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="42" t="n">
+        <v>0.78125</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="42" t="n">
+        <v>0.520833333333333</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="42" t="n">
+        <v>0.583333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:J1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="true" showErrorMessage="true" showInputMessage="false" sqref="D2:J2" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>